<commit_message>
added regression plot, modified appearance of scatter plots
</commit_message>
<xml_diff>
--- a/regression_analysis.xlsx
+++ b/regression_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balu\Nextcloud\Documents\MA\Code\OpenSimOutputToMAT-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1A447-0ED9-47A1-A5E8-B000AD09EFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1F6CCE-D168-4D97-B34C-882A915606A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="-18000" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,21 +240,21 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R50" sqref="R50"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2290,7 +2290,7 @@
         <v>1.7504310752648913E-3</v>
       </c>
       <c r="R43" s="1">
-        <v>1.6079182363537531E-2</v>
+        <v>1.60791823635375E-2</v>
       </c>
       <c r="S43" s="1">
         <v>6.130467578064995E-2</v>
@@ -2319,7 +2319,7 @@
         <v>1.0393608433673544E-2</v>
       </c>
       <c r="R44" s="2">
-        <v>-4.6930390357782736E-2</v>
+        <v>-4.6930390357782702E-2</v>
       </c>
       <c r="S44" s="2">
         <v>-6.9718984949400722E-3</v>

</xml_diff>

<commit_message>
fixed creation of muscle groups and their scatter plots
</commit_message>
<xml_diff>
--- a/regression_analysis.xlsx
+++ b/regression_analysis.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balu\Nextcloud\Documents\MA\Code\OpenSimOutputToMAT-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1F6CCE-D168-4D97-B34C-882A915606A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B7D17-FE36-4AFD-9789-C11634E19147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="-18000" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HCF" sheetId="1" r:id="rId1"/>
+    <sheet name="KCF" sheetId="2" r:id="rId2"/>
+    <sheet name="glut min" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>X_1</t>
   </si>
@@ -156,6 +158,12 @@
   </si>
   <si>
     <t>Residuen</t>
+  </si>
+  <si>
+    <t>KCF</t>
+  </si>
+  <si>
+    <t>Glut min</t>
   </si>
 </sst>
 </file>
@@ -320,7 +328,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$27</c:f>
+              <c:f>HCF!$H$2:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -407,7 +415,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$51:$O$76</c:f>
+              <c:f>HCF!$O$51:$O$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -644,7 +652,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$27</c:f>
+              <c:f>HCF!$I$2:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
@@ -731,7 +739,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$51:$O$76</c:f>
+              <c:f>HCF!$O$51:$O$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1296,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2639,4 +2647,642 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A90CE2-368A-426F-91D3-A0D3271E0A90}">
+  <dimension ref="B1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C2" s="5">
+        <v>128.9</v>
+      </c>
+      <c r="D2" s="5">
+        <v>42.2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C3" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>27.2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="5">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="5">
+        <v>137</v>
+      </c>
+      <c r="D5" s="5">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E5" s="5">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C6" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>12.7</v>
+      </c>
+      <c r="E6" s="5">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="5">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="D7" s="5">
+        <v>52.3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="5">
+        <v>129</v>
+      </c>
+      <c r="D8" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="D9" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="E9" s="5">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="D10" s="5">
+        <v>42.1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C11" s="5">
+        <v>145.5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="5">
+        <v>128.9</v>
+      </c>
+      <c r="D12" s="5">
+        <v>42.2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>27.2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C14" s="5">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="5">
+        <v>137</v>
+      </c>
+      <c r="D15" s="5">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E15" s="5">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D16" s="5">
+        <v>12.7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="5">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="D17" s="5">
+        <v>52.3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="5">
+        <v>129</v>
+      </c>
+      <c r="D18" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="E18" s="5">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="D19" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="E19" s="5">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="D20" s="5">
+        <v>42.1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="5">
+        <v>145.5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>18</v>
+      </c>
+      <c r="E21" s="5">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="5">
+        <v>120.1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>27.3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="5">
+        <v>126.2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="5">
+        <v>125.8</v>
+      </c>
+      <c r="D24" s="5">
+        <v>26.1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="5">
+        <v>126</v>
+      </c>
+      <c r="D25" s="5">
+        <v>13.3</v>
+      </c>
+      <c r="E25" s="5">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" s="5">
+        <v>124.6</v>
+      </c>
+      <c r="D26" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="E26" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="5">
+        <v>124.8</v>
+      </c>
+      <c r="D27" s="5">
+        <v>28.7</v>
+      </c>
+      <c r="E27" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D7C3B5-13B6-4360-A339-3F6900F12A60}">
+  <dimension ref="B1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C2" s="5">
+        <v>128.9</v>
+      </c>
+      <c r="D2" s="5">
+        <v>42.2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C3" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>27.2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="5">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="5">
+        <v>137</v>
+      </c>
+      <c r="D5" s="5">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E5" s="5">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C6" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>12.7</v>
+      </c>
+      <c r="E6" s="5">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="5">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="D7" s="5">
+        <v>52.3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="5">
+        <v>129</v>
+      </c>
+      <c r="D8" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="D9" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="E9" s="5">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="D10" s="5">
+        <v>42.1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C11" s="5">
+        <v>145.5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="5">
+        <v>128.9</v>
+      </c>
+      <c r="D12" s="5">
+        <v>42.2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>27.2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C14" s="5">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="5">
+        <v>137</v>
+      </c>
+      <c r="D15" s="5">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E15" s="5">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D16" s="5">
+        <v>12.7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="5">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="D17" s="5">
+        <v>52.3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="5">
+        <v>129</v>
+      </c>
+      <c r="D18" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="E18" s="5">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="D19" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="E19" s="5">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="D20" s="5">
+        <v>42.1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="5">
+        <v>145.5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>18</v>
+      </c>
+      <c r="E21" s="5">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="5">
+        <v>120.1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>27.3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="5">
+        <v>126.2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="5">
+        <v>125.8</v>
+      </c>
+      <c r="D24" s="5">
+        <v>26.1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="5">
+        <v>126</v>
+      </c>
+      <c r="D25" s="5">
+        <v>13.3</v>
+      </c>
+      <c r="E25" s="5">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" s="5">
+        <v>124.6</v>
+      </c>
+      <c r="D26" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="E26" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="5">
+        <v>124.8</v>
+      </c>
+      <c r="D27" s="5">
+        <v>28.7</v>
+      </c>
+      <c r="E27" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added SPM of muscles normalised to BW
</commit_message>
<xml_diff>
--- a/regression_analysis.xlsx
+++ b/regression_analysis.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balu\Nextcloud\Documents\MA\Code\OpenSimOutputToMAT-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B7D17-FE36-4AFD-9789-C11634E19147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A51CF65-7E7D-41BC-AD9B-64E527731EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HCF" sheetId="1" r:id="rId1"/>
     <sheet name="KCF" sheetId="2" r:id="rId2"/>
-    <sheet name="glut min" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
   <si>
     <t>X_1</t>
   </si>
@@ -163,7 +162,7 @@
     <t>KCF</t>
   </si>
   <si>
-    <t>Glut min</t>
+    <t>Schätzung für KCF</t>
   </si>
 </sst>
 </file>
@@ -246,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -263,6 +262,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -928,6 +935,330 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>NSA Residuenplot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>KCF!$C$2:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>128.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>139.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>139.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>145.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>134.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>139.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>135.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>139.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>130.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>126.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>125.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>124.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>124.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>KCF!$I$25:$I$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.1243223166122469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.15924409396619144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1188190873450568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.68312723562041899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.1033135152785416</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1603989008473379</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16301401813025773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.2113328387351761</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.84296724190452821</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.3922493386423902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.23506435658843294</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.491675267457822E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.669296047595477</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.0952312436231688</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.21880335711437127</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.78115963522195209</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.28087283279296749</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.72276206086487349</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2671730899871392E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25192315435141932</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.85551572199809289</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.42418569111247617</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.8482523166668825</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.341771650078956</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.28991311090044292</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.75843220797826483</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2B55-4756-8CAA-D744C480E73A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2112506256"/>
+        <c:axId val="2112514896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2112506256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>NSA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2112514896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2112514896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Residuen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2112506256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -997,6 +1328,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAAC9DF8-EA19-DB5D-E300-323D34DFF990}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1305,7 +1677,7 @@
   <dimension ref="A1:V76"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1048576"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2651,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A90CE2-368A-426F-91D3-A0D3271E0A90}">
-  <dimension ref="B1:E27"/>
+  <dimension ref="B1:O52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2663,7 +3035,7 @@
     <col min="4" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>41</v>
       </c>
@@ -2676,8 +3048,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="5">
+        <v>6.4318788273508103</v>
+      </c>
       <c r="C2" s="5">
         <v>128.9</v>
       </c>
@@ -2688,7 +3066,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B3" s="5">
+        <v>5.44441351714429</v>
+      </c>
       <c r="C3" s="5">
         <v>134.1</v>
       </c>
@@ -2698,8 +3079,15 @@
       <c r="E3" s="5">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="5">
+        <v>7.0755203181297501</v>
+      </c>
       <c r="C4" s="5">
         <v>140.30000000000001</v>
       </c>
@@ -2709,8 +3097,17 @@
       <c r="E4" s="5">
         <v>49.4</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.42133043146253152</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="5">
+        <v>5.08566368146671</v>
+      </c>
       <c r="C5" s="5">
         <v>137</v>
       </c>
@@ -2720,8 +3117,17 @@
       <c r="E5" s="5">
         <v>37.700000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.17751933247640295</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B6" s="5">
+        <v>4.7964451962038597</v>
+      </c>
       <c r="C6" s="5">
         <v>139.30000000000001</v>
       </c>
@@ -2731,8 +3137,17 @@
       <c r="E6" s="5">
         <v>45.8</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.14324930466291974</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B7" s="5">
+        <v>6.8266932831903402</v>
+      </c>
       <c r="C7" s="5">
         <v>135.19999999999999</v>
       </c>
@@ -2742,8 +3157,17 @@
       <c r="E7" s="5">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.85133186092910684</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5">
+        <v>5.4762647807990499</v>
+      </c>
       <c r="C8" s="5">
         <v>129</v>
       </c>
@@ -2753,8 +3177,17 @@
       <c r="E8" s="5">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B9" s="5">
+        <v>4.7112028804681403</v>
+      </c>
       <c r="C9" s="5">
         <v>139.69999999999999</v>
       </c>
@@ -2765,7 +3198,10 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="5">
+        <v>4.5613915516479304</v>
+      </c>
       <c r="C10" s="5">
         <v>130.6</v>
       </c>
@@ -2775,8 +3211,14 @@
       <c r="E10" s="5">
         <v>50.2</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B11" s="5">
+        <v>5.8605529925142203</v>
+      </c>
       <c r="C11" s="5">
         <v>145.5</v>
       </c>
@@ -2786,8 +3228,27 @@
       <c r="E11" s="5">
         <v>47.3</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B12" s="5">
+        <v>5.0724921541501304</v>
+      </c>
       <c r="C12" s="5">
         <v>128.9</v>
       </c>
@@ -2797,8 +3258,29 @@
       <c r="E12" s="5">
         <v>10.1</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12">
+        <v>3.754299999841944</v>
+      </c>
+      <c r="J12" s="12">
+        <v>3.754299999841944</v>
+      </c>
+      <c r="K12" s="12">
+        <v>5.1800171695968009</v>
+      </c>
+      <c r="L12" s="12">
+        <v>3.2060865142186257E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B13" s="5">
+        <v>5.6985743637850597</v>
+      </c>
       <c r="C13" s="5">
         <v>134.1</v>
       </c>
@@ -2808,8 +3290,25 @@
       <c r="E13" s="5">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="12">
+        <v>24</v>
+      </c>
+      <c r="I13" s="12">
+        <v>17.394382498392385</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0.72476593743301609</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="5">
+        <v>7.6259972783801704</v>
+      </c>
       <c r="C14" s="5">
         <v>140.30000000000001</v>
       </c>
@@ -2819,8 +3318,23 @@
       <c r="E14" s="5">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="G14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="13">
+        <v>25</v>
+      </c>
+      <c r="I14" s="13">
+        <v>21.148682498234329</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="5">
+        <v>4.6735596734639602</v>
+      </c>
       <c r="C15" s="5">
         <v>137</v>
       </c>
@@ -2831,7 +3345,10 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B16" s="5">
+        <v>5.68095535436803</v>
+      </c>
       <c r="C16" s="5">
         <v>139.30000000000001</v>
       </c>
@@ -2841,8 +3358,36 @@
       <c r="E16" s="5">
         <v>27.8</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B17" s="5">
+        <v>4.8851347471210502</v>
+      </c>
       <c r="C17" s="5">
         <v>135.19999999999999</v>
       </c>
@@ -2852,8 +3397,38 @@
       <c r="E17" s="5">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="12">
+        <v>-2.0323342273268832</v>
+      </c>
+      <c r="I17" s="12">
+        <v>3.3400829315673151</v>
+      </c>
+      <c r="J17" s="12">
+        <v>-0.608468193444892</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0.54859306269530017</v>
+      </c>
+      <c r="L17" s="12">
+        <v>-8.925926585506982</v>
+      </c>
+      <c r="M17" s="12">
+        <v>4.8612581308532166</v>
+      </c>
+      <c r="N17" s="12">
+        <v>-8.925926585506982</v>
+      </c>
+      <c r="O17" s="12">
+        <v>4.8612581308532166</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="5">
+        <v>5.5941235954617596</v>
+      </c>
       <c r="C18" s="5">
         <v>129</v>
       </c>
@@ -2863,8 +3438,38 @@
       <c r="E18" s="5">
         <v>23.7</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="13">
+        <v>5.6942519302292056E-2</v>
+      </c>
+      <c r="I18" s="13">
+        <v>2.5019065151714884E-2</v>
+      </c>
+      <c r="J18" s="13">
+        <v>2.2759651072889526</v>
+      </c>
+      <c r="K18" s="13">
+        <v>3.2060865142186083E-2</v>
+      </c>
+      <c r="L18" s="13">
+        <v>5.3057067223898496E-3</v>
+      </c>
+      <c r="M18" s="13">
+        <v>0.10857933188219426</v>
+      </c>
+      <c r="N18" s="13">
+        <v>5.3057067223898496E-3</v>
+      </c>
+      <c r="O18" s="13">
+        <v>0.10857933188219426</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B19" s="5">
+        <v>6.6452977800681898</v>
+      </c>
       <c r="C19" s="5">
         <v>139.69999999999999</v>
       </c>
@@ -2875,7 +3480,10 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B20" s="5">
+        <v>5.41703052445233</v>
+      </c>
       <c r="C20" s="5">
         <v>130.6</v>
       </c>
@@ -2886,7 +3494,10 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B21" s="5">
+        <v>6.5047254855080299</v>
+      </c>
       <c r="C21" s="5">
         <v>145.5</v>
       </c>
@@ -2897,7 +3508,10 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B22" s="5">
+        <v>3.9509466188803</v>
+      </c>
       <c r="C22" s="5">
         <v>120.1</v>
       </c>
@@ -2907,8 +3521,14 @@
       <c r="E22" s="5">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="5">
+        <v>5.5779973997348504</v>
+      </c>
       <c r="C23" s="5">
         <v>126.2</v>
       </c>
@@ -2919,7 +3539,10 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B24" s="5">
+        <v>5.9792870175683399</v>
+      </c>
       <c r="C24" s="5">
         <v>125.8</v>
       </c>
@@ -2929,8 +3552,20 @@
       <c r="E24" s="5">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B25" s="5">
+        <v>3.8006515546829598</v>
+      </c>
       <c r="C25" s="5">
         <v>126</v>
       </c>
@@ -2940,8 +3575,20 @@
       <c r="E25" s="5">
         <v>26.9</v>
       </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G25" s="12">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12">
+        <v>5.3075565107385634</v>
+      </c>
+      <c r="I25" s="12">
+        <v>1.1243223166122469</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B26" s="5">
+        <v>5.3526167886391498</v>
+      </c>
       <c r="C26" s="5">
         <v>124.6</v>
       </c>
@@ -2951,8 +3598,20 @@
       <c r="E26" s="5">
         <v>22.2</v>
       </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="G26" s="12">
+        <v>2</v>
+      </c>
+      <c r="H26" s="12">
+        <v>5.6036576111104814</v>
+      </c>
+      <c r="I26" s="12">
+        <v>-0.15924409396619144</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B27" s="5">
+        <v>5.8325243895774301</v>
+      </c>
       <c r="C27" s="5">
         <v>124.8</v>
       </c>
@@ -2962,327 +3621,282 @@
       <c r="E27" s="5">
         <v>4.9000000000000004</v>
       </c>
+      <c r="G27" s="12">
+        <v>3</v>
+      </c>
+      <c r="H27" s="12">
+        <v>5.9567012307846934</v>
+      </c>
+      <c r="I27" s="12">
+        <v>1.1188190873450568</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G28" s="12">
+        <v>4</v>
+      </c>
+      <c r="H28" s="12">
+        <v>5.768790917087129</v>
+      </c>
+      <c r="I28" s="12">
+        <v>-0.68312723562041899</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G29" s="12">
+        <v>5</v>
+      </c>
+      <c r="H29" s="12">
+        <v>5.8997587114824013</v>
+      </c>
+      <c r="I29" s="12">
+        <v>-1.1033135152785416</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G30" s="12">
+        <v>6</v>
+      </c>
+      <c r="H30" s="12">
+        <v>5.6662943823430023</v>
+      </c>
+      <c r="I30" s="12">
+        <v>1.1603989008473379</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G31" s="12">
+        <v>7</v>
+      </c>
+      <c r="H31" s="12">
+        <v>5.3132507626687921</v>
+      </c>
+      <c r="I31" s="12">
+        <v>0.16301401813025773</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G32" s="12">
+        <v>8</v>
+      </c>
+      <c r="H32" s="12">
+        <v>5.9225357192033163</v>
+      </c>
+      <c r="I32" s="12">
+        <v>-1.2113328387351761</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G33" s="12">
+        <v>9</v>
+      </c>
+      <c r="H33" s="12">
+        <v>5.4043587935524586</v>
+      </c>
+      <c r="I33" s="12">
+        <v>-0.84296724190452821</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G34" s="12">
+        <v>10</v>
+      </c>
+      <c r="H34" s="12">
+        <v>6.2528023311566105</v>
+      </c>
+      <c r="I34" s="12">
+        <v>-0.3922493386423902</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G35" s="12">
+        <v>11</v>
+      </c>
+      <c r="H35" s="12">
+        <v>5.3075565107385634</v>
+      </c>
+      <c r="I35" s="12">
+        <v>-0.23506435658843294</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G36" s="12">
+        <v>12</v>
+      </c>
+      <c r="H36" s="12">
+        <v>5.6036576111104814</v>
+      </c>
+      <c r="I36" s="12">
+        <v>9.491675267457822E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G37" s="12">
+        <v>13</v>
+      </c>
+      <c r="H37" s="12">
+        <v>5.9567012307846934</v>
+      </c>
+      <c r="I37" s="12">
+        <v>1.669296047595477</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G38" s="12">
+        <v>14</v>
+      </c>
+      <c r="H38" s="12">
+        <v>5.768790917087129</v>
+      </c>
+      <c r="I38" s="12">
+        <v>-1.0952312436231688</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G39" s="12">
+        <v>15</v>
+      </c>
+      <c r="H39" s="12">
+        <v>5.8997587114824013</v>
+      </c>
+      <c r="I39" s="12">
+        <v>-0.21880335711437127</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G40" s="12">
+        <v>16</v>
+      </c>
+      <c r="H40" s="12">
+        <v>5.6662943823430023</v>
+      </c>
+      <c r="I40" s="12">
+        <v>-0.78115963522195209</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G41" s="12">
+        <v>17</v>
+      </c>
+      <c r="H41" s="12">
+        <v>5.3132507626687921</v>
+      </c>
+      <c r="I41" s="12">
+        <v>0.28087283279296749</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G42" s="12">
+        <v>18</v>
+      </c>
+      <c r="H42" s="12">
+        <v>5.9225357192033163</v>
+      </c>
+      <c r="I42" s="12">
+        <v>0.72276206086487349</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G43" s="12">
+        <v>19</v>
+      </c>
+      <c r="H43" s="12">
+        <v>5.4043587935524586</v>
+      </c>
+      <c r="I43" s="12">
+        <v>1.2671730899871392E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G44" s="12">
+        <v>20</v>
+      </c>
+      <c r="H44" s="12">
+        <v>6.2528023311566105</v>
+      </c>
+      <c r="I44" s="12">
+        <v>0.25192315435141932</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G45" s="12">
+        <v>21</v>
+      </c>
+      <c r="H45" s="12">
+        <v>4.8064623408783929</v>
+      </c>
+      <c r="I45" s="12">
+        <v>-0.85551572199809289</v>
+      </c>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G46" s="12">
+        <v>22</v>
+      </c>
+      <c r="H46" s="12">
+        <v>5.1538117086223743</v>
+      </c>
+      <c r="I46" s="12">
+        <v>0.42418569111247617</v>
+      </c>
+    </row>
+    <row r="47" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G47" s="12">
+        <v>23</v>
+      </c>
+      <c r="H47" s="12">
+        <v>5.1310347009014574</v>
+      </c>
+      <c r="I47" s="12">
+        <v>0.8482523166668825</v>
+      </c>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G48" s="12">
+        <v>24</v>
+      </c>
+      <c r="H48" s="12">
+        <v>5.1424232047619158</v>
+      </c>
+      <c r="I48" s="12">
+        <v>-1.341771650078956</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G49" s="12">
+        <v>25</v>
+      </c>
+      <c r="H49" s="12">
+        <v>5.0627036777387069</v>
+      </c>
+      <c r="I49" s="12">
+        <v>0.28991311090044292</v>
+      </c>
+    </row>
+    <row r="50" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G50" s="13">
+        <v>26</v>
+      </c>
+      <c r="H50" s="13">
+        <v>5.0740921815991653</v>
+      </c>
+      <c r="I50" s="13">
+        <v>0.75843220797826483</v>
+      </c>
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D7C3B5-13B6-4360-A339-3F6900F12A60}">
-  <dimension ref="B1:E27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="5">
-        <v>128.9</v>
-      </c>
-      <c r="D2" s="5">
-        <v>42.2</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C3" s="5">
-        <v>134.1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>27.2</v>
-      </c>
-      <c r="E3" s="5">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C4" s="5">
-        <v>140.30000000000001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5">
-        <v>49.4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C5" s="5">
-        <v>137</v>
-      </c>
-      <c r="D5" s="5">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="E5" s="5">
-        <v>37.700000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C6" s="5">
-        <v>139.30000000000001</v>
-      </c>
-      <c r="D6" s="5">
-        <v>12.7</v>
-      </c>
-      <c r="E6" s="5">
-        <v>45.8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C7" s="5">
-        <v>135.19999999999999</v>
-      </c>
-      <c r="D7" s="5">
-        <v>52.3</v>
-      </c>
-      <c r="E7" s="5">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C8" s="5">
-        <v>129</v>
-      </c>
-      <c r="D8" s="5">
-        <v>22.2</v>
-      </c>
-      <c r="E8" s="5">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C9" s="5">
-        <v>139.69999999999999</v>
-      </c>
-      <c r="D9" s="5">
-        <v>14.6</v>
-      </c>
-      <c r="E9" s="5">
-        <v>34.1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C10" s="5">
-        <v>130.6</v>
-      </c>
-      <c r="D10" s="5">
-        <v>42.1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>50.2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C11" s="5">
-        <v>145.5</v>
-      </c>
-      <c r="D11" s="5">
-        <v>18</v>
-      </c>
-      <c r="E11" s="5">
-        <v>47.3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C12" s="5">
-        <v>128.9</v>
-      </c>
-      <c r="D12" s="5">
-        <v>42.2</v>
-      </c>
-      <c r="E12" s="5">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C13" s="5">
-        <v>134.1</v>
-      </c>
-      <c r="D13" s="5">
-        <v>27.2</v>
-      </c>
-      <c r="E13" s="5">
-        <v>21.3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C14" s="5">
-        <v>140.30000000000001</v>
-      </c>
-      <c r="D14" s="5">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5">
-        <v>19.399999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C15" s="5">
-        <v>137</v>
-      </c>
-      <c r="D15" s="5">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="E15" s="5">
-        <v>17.7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C16" s="5">
-        <v>139.30000000000001</v>
-      </c>
-      <c r="D16" s="5">
-        <v>12.7</v>
-      </c>
-      <c r="E16" s="5">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C17" s="5">
-        <v>135.19999999999999</v>
-      </c>
-      <c r="D17" s="5">
-        <v>52.3</v>
-      </c>
-      <c r="E17" s="5">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="5">
-        <v>129</v>
-      </c>
-      <c r="D18" s="5">
-        <v>22.2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="5">
-        <v>139.69999999999999</v>
-      </c>
-      <c r="D19" s="5">
-        <v>14.6</v>
-      </c>
-      <c r="E19" s="5">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C20" s="5">
-        <v>130.6</v>
-      </c>
-      <c r="D20" s="5">
-        <v>42.1</v>
-      </c>
-      <c r="E20" s="5">
-        <v>25.2</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C21" s="5">
-        <v>145.5</v>
-      </c>
-      <c r="D21" s="5">
-        <v>18</v>
-      </c>
-      <c r="E21" s="5">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="5">
-        <v>120.1</v>
-      </c>
-      <c r="D22" s="5">
-        <v>27.3</v>
-      </c>
-      <c r="E22" s="5">
-        <v>25.8</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C23" s="5">
-        <v>126.2</v>
-      </c>
-      <c r="D23" s="5">
-        <v>20.2</v>
-      </c>
-      <c r="E23" s="5">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="5">
-        <v>125.8</v>
-      </c>
-      <c r="D24" s="5">
-        <v>26.1</v>
-      </c>
-      <c r="E24" s="5">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C25" s="5">
-        <v>126</v>
-      </c>
-      <c r="D25" s="5">
-        <v>13.3</v>
-      </c>
-      <c r="E25" s="5">
-        <v>26.9</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C26" s="5">
-        <v>124.6</v>
-      </c>
-      <c r="D26" s="5">
-        <v>17.7</v>
-      </c>
-      <c r="E26" s="5">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C27" s="5">
-        <v>124.8</v>
-      </c>
-      <c r="D27" s="5">
-        <v>28.7</v>
-      </c>
-      <c r="E27" s="5">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added calculation of walking velocity
</commit_message>
<xml_diff>
--- a/regression_analysis.xlsx
+++ b/regression_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balu\Nextcloud\Documents\MA\Code\OpenSimOutputToMAT-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A51CF65-7E7D-41BC-AD9B-64E527731EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B113820A-7390-44AD-9A8D-93C3C341D5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HCF" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
   <si>
     <t>X_1</t>
   </si>
@@ -162,14 +162,14 @@
     <t>KCF</t>
   </si>
   <si>
-    <t>Schätzung für KCF</t>
+    <t>Pred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -245,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -270,6 +270,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -942,30 +944,70 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="103"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="3"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>NSA Residuenplot</a:t>
+              <a:rPr lang="de-DE">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Diagrammtitel</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -977,180 +1019,261 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.1911377651803252E-2"/>
+                  <c:y val="-8.8277456647398847E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>KCF!$C$2:$C$27</c:f>
+              <c:f>HCF!$F$2:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>128.9</c:v>
+                  <c:v>7.794902788576854</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>134.1</c:v>
+                  <c:v>5.6145824835581086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140.30000000000001</c:v>
+                  <c:v>5.7985229229993012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137</c:v>
+                  <c:v>4.8669137545727672</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>139.30000000000001</c:v>
+                  <c:v>4.1979434476288571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>135.19999999999999</c:v>
+                  <c:v>8.4730851492894086</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>129</c:v>
+                  <c:v>5.5983628800740126</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>139.69999999999999</c:v>
+                  <c:v>4.5890702146240399</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130.6</c:v>
+                  <c:v>5.329088655857686</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>145.5</c:v>
+                  <c:v>5.0168597960424659</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>128.9</c:v>
+                  <c:v>6.1967192914215525</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>134.1</c:v>
+                  <c:v>5.4691418184599261</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>140.30000000000001</c:v>
+                  <c:v>5.2510399715547376</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>137</c:v>
+                  <c:v>4.9792462160437942</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>139.30000000000001</c:v>
+                  <c:v>5.0076139263769601</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>135.19999999999999</c:v>
+                  <c:v>6.53283850341451</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>129</c:v>
+                  <c:v>5.3579745918742701</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>139.69999999999999</c:v>
+                  <c:v>5.1957226906850584</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>130.6</c:v>
+                  <c:v>6.9160996288951475</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>145.5</c:v>
+                  <c:v>5.6366487476458111</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>120.1</c:v>
+                  <c:v>4.9615063166628772</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>126.2</c:v>
+                  <c:v>5.5765260152581746</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>125.8</c:v>
+                  <c:v>6.7429396312826997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>126</c:v>
+                  <c:v>4.3317628745786223</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>124.6</c:v>
+                  <c:v>5.9371153246213719</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>124.8</c:v>
+                  <c:v>5.8278694844035899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>KCF!$I$25:$I$50</c:f>
+              <c:f>HCF!$K$2:$K$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1.1243223166122469</c:v>
+                  <c:v>6.8853948026665632</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.15924409396619144</c:v>
+                  <c:v>6.1948694029538416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1188190873450568</c:v>
+                  <c:v>4.2341327850929344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.68312723562041899</c:v>
+                  <c:v>5.6605714234325442</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.1033135152785416</c:v>
+                  <c:v>4.5127879312995169</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1603989008473379</c:v>
+                  <c:v>7.3093038035180804</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16301401813025773</c:v>
+                  <c:v>5.8248780033450664</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.2113328387351761</c:v>
+                  <c:v>4.9519120047560508</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.84296724190452821</c:v>
+                  <c:v>5.3917189276585527</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.3922493386423902</c:v>
+                  <c:v>4.7971998309057433</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.23506435658843294</c:v>
+                  <c:v>6.5816154681622558</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.491675267457822E-2</c:v>
+                  <c:v>5.7392004011973805</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.669296047595477</c:v>
+                  <c:v>5.1454707886058557</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.0952312436231688</c:v>
+                  <c:v>6.2681300924411598</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.21880335711437127</c:v>
+                  <c:v>5.0595907334072701</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.78115963522195209</c:v>
+                  <c:v>6.8536348017616193</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28087283279296749</c:v>
+                  <c:v>5.3692090015886045</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.72276206086487349</c:v>
+                  <c:v>5.5594706737646655</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2671730899871392E-2</c:v>
+                  <c:v>6.1511672639193211</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.25192315435141932</c:v>
+                  <c:v>5.4655143668152197</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.85551572199809289</c:v>
+                  <c:v>5.3407985904139679</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.42418569111247617</c:v>
+                  <c:v>5.691620168984505</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.8482523166668825</c:v>
+                  <c:v>6.0813751107260234</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-1.341771650078956</c:v>
+                  <c:v>4.8585442218463228</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.28991311090044292</c:v>
+                  <c:v>5.1510060010266487</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.75843220797826483</c:v>
+                  <c:v>6.1209805261129038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1158,7 +1281,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2B55-4756-8CAA-D744C480E73A}"/>
+              <c16:uniqueId val="{00000000-39BE-4190-83AB-75B05D6E85CE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1170,75 +1293,255 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2112506256"/>
-        <c:axId val="2112514896"/>
+        <c:axId val="1261563280"/>
+        <c:axId val="1261559920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2112506256"/>
+        <c:axId val="1261563280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>NSA</a:t>
+                  <a:t>Actual HCF</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112514896"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261559920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2112514896"/>
+        <c:axId val="1261559920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Residuen</a:t>
+                  <a:t>Predicted</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> (NSA, AVA, TT)</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112506256"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261563280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1251,12 +1554,1737 @@
     </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.546863799773465E-2"/>
+                  <c:y val="-0.10191464821222607"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HCF!$F$2:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.794902788576854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6145824835581086</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7985229229993012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8669137545727672</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1979434476288571</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4730851492894086</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5983628800740126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5890702146240399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.329088655857686</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0168597960424659</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.1967192914215525</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.4691418184599261</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.2510399715547376</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9792462160437942</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0076139263769601</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.53283850341451</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.3579745918742701</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.1957226906850584</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.9160996288951475</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.6366487476458111</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.9615063166628772</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.5765260152581746</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.7429396312826997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.3317628745786223</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.9371153246213719</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.8278694844035899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HCF!$L$2:$L$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>6.8720480631900536</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1245720316652061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2200926687048304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6304026512335117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.498968855278572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1738977702112079</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8664296396814706</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8878119103039781</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5179265345221378</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.663609362721127</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.6025366189264396</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7203048652697852</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0286270014956722</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.1694255397607396</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.984089454953077</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.769630603815787</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4621624732860496</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4268347988312069</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.1917051451811727</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.2565345401010779</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.6028939082583689</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.7890457815372827</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.1601692285223519</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0315606423800592</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.3284755091011702</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.2203415274702536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A63E-4B20-9EB9-395B815C3E51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1261563280"/>
+        <c:axId val="1261559920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1261563280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Actual HCF</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261559920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1261559920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Predicted</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> (AVA, TT)</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1261563280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1333,30 +3361,25 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390129</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>173434</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>517922</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>178196</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagramm 4">
+        <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAAC9DF8-EA19-DB5D-E300-323D34DFF990}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB69696D-50BE-9CB4-5DFA-E6E799BD6B92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1368,7 +3391,45 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>422275</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>46831</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A75C5A2-EB3B-4FEA-B741-CCF93EE01815}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1677,10 +3738,10 @@
   <dimension ref="A1:V76"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="4.1796875" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
@@ -1697,7 +3758,7 @@
     <col min="21" max="21" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1716,8 +3777,14 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1736,11 +3803,19 @@
       <c r="J2" s="5">
         <v>-42.1</v>
       </c>
+      <c r="K2">
+        <f>$N$19*G2+$N$20*H2+I2*$N$21+$N$18</f>
+        <v>6.8853948026665632</v>
+      </c>
+      <c r="L2">
+        <f>$N$43*H2+I2*$N$44+$N$42</f>
+        <v>6.8720480631900536</v>
+      </c>
       <c r="M2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1759,8 +3834,16 @@
       <c r="J3" s="5">
         <v>-20.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <f t="shared" ref="K3:L27" si="0">$N$19*G3+$N$20*H3+I3*$N$21+$N$18</f>
+        <v>6.1948694029538416</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L27" si="1">$N$43*H3+I3*$N$44+$N$42</f>
+        <v>6.1245720316652061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1779,12 +3862,20 @@
       <c r="J4" s="5">
         <v>41.4</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>4.2341327850929344</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>4.2200926687048304</v>
+      </c>
       <c r="M4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1803,6 +3894,14 @@
       <c r="J5" s="5">
         <v>1.4000000000000057</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>5.6605714234325442</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>5.6304026512335117</v>
+      </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1810,7 +3909,7 @@
         <v>0.76256961395444722</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1829,6 +3928,14 @@
       <c r="J6" s="5">
         <v>33.099999999999994</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>4.5127879312995169</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>4.498968855278572</v>
+      </c>
       <c r="M6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +3943,7 @@
         <v>0.58151241612663473</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1855,6 +3962,14 @@
       <c r="J7" s="5">
         <v>-48.9</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>7.3093038035180804</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>7.1738977702112079</v>
+      </c>
       <c r="M7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1862,7 +3977,7 @@
         <v>0.52444592741663043</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1881,6 +3996,14 @@
       <c r="J8" s="5">
         <v>-13.5</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>5.8248780033450664</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>5.8664296396814706</v>
+      </c>
       <c r="M8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1888,7 +4011,7 @@
         <v>0.68263716178210532</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1907,6 +4030,14 @@
       <c r="J9" s="5">
         <v>19.5</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>4.9519120047560508</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>4.8878119103039781</v>
+      </c>
       <c r="M9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1914,7 +4045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1933,8 +4064,16 @@
       <c r="J10" s="5">
         <v>8.1000000000000014</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>5.3917189276585527</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>5.5179265345221378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" thickBot="1">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1953,11 +4092,19 @@
       <c r="J11" s="5">
         <v>29.299999999999997</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>4.7971998309057433</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>4.663609362721127</v>
+      </c>
       <c r="M11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1975,6 +4122,14 @@
       </c>
       <c r="J12" s="5">
         <v>-32.1</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>6.5816154681622558</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>6.6025366189264396</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3" t="s">
@@ -1993,7 +4148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2012,6 +4167,14 @@
       <c r="J13" s="5">
         <v>-5.8999999999999986</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>5.7392004011973805</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>5.7203048652697852</v>
+      </c>
       <c r="M13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2034,7 +4197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2053,6 +4216,14 @@
       <c r="J14" s="5">
         <v>11.399999999999999</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>5.1454707886058557</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>5.0286270014956722</v>
+      </c>
       <c r="M14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +4239,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" ht="15" thickBot="1">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2086,6 +4257,14 @@
       </c>
       <c r="J15" s="5">
         <v>-18.599999999999998</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>6.2681300924411598</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>6.1694255397607396</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>16</v>
@@ -2100,7 +4279,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" ht="15" thickBot="1">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2119,8 +4298,16 @@
       <c r="J16" s="5">
         <v>15.100000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>5.0595907334072701</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>4.984089454953077</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2138,6 +4325,14 @@
       </c>
       <c r="J17" s="5">
         <v>-33.9</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>6.8536348017616193</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>6.769630603815787</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3" t="s">
@@ -2165,7 +4360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2184,6 +4379,14 @@
       <c r="J18" s="5">
         <v>1.5</v>
       </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>5.3692090015886045</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>5.4621624732860496</v>
+      </c>
       <c r="M18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2212,7 +4415,7 @@
         <v>8.9685142270423697</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2231,6 +4434,14 @@
       <c r="J19" s="5">
         <v>-0.5</v>
       </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>5.5594706737646655</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>5.4268347988312069</v>
+      </c>
       <c r="M19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +4471,7 @@
       </c>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2279,6 +4490,14 @@
       <c r="J20" s="5">
         <v>-16.900000000000002</v>
       </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>6.1511672639193211</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>6.1917051451811727</v>
+      </c>
       <c r="M20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2307,7 +4526,7 @@
         <v>6.3122937720888311E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:22" ht="15" thickBot="1">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2326,6 +4545,14 @@
       <c r="J21" s="5">
         <v>7.3000000000000007</v>
       </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>5.4655143668152197</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>5.2565345401010779</v>
+      </c>
       <c r="M21" s="2" t="s">
         <v>4</v>
       </c>
@@ -2354,7 +4581,7 @@
         <v>-8.5140490642037596E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2373,8 +4600,16 @@
       <c r="J22" s="5">
         <v>-1.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>5.3407985904139679</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>5.6028939082583689</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2393,8 +4628,16 @@
       <c r="J23" s="5">
         <v>-11.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>5.691620168984505</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>5.7890457815372827</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2413,8 +4656,16 @@
       <c r="J24" s="5">
         <v>-22.700000000000003</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>6.0813751107260234</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>6.1601692285223519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2433,8 +4684,16 @@
       <c r="J25" s="5">
         <v>13.599999999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>4.8585442218463228</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>5.0315606423800592</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2453,11 +4712,19 @@
       <c r="J26" s="5">
         <v>4.5</v>
       </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>5.1510060010266487</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>5.3284755091011702</v>
+      </c>
       <c r="M26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:22" ht="15" thickBot="1">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2476,14 +4743,22 @@
       <c r="J27" s="5">
         <v>-23.799999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>6.1209805261129038</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>6.2203415274702536</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
       <c r="M28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22">
       <c r="M29" s="10" t="s">
         <v>36</v>
       </c>
@@ -2491,7 +4766,7 @@
         <v>0.75372446319004371</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22">
       <c r="M30" s="10" t="s">
         <v>33</v>
       </c>
@@ -2499,7 +4774,7 @@
         <v>0.5681005664111195</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22">
       <c r="M31" s="10" t="s">
         <v>35</v>
       </c>
@@ -2507,7 +4782,7 @@
         <v>0.53054409392512991</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22">
       <c r="M32" s="10" t="s">
         <v>32</v>
       </c>
@@ -2515,7 +4790,7 @@
         <v>0.6782462135355104</v>
       </c>
     </row>
-    <row r="33" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="13:21" ht="15" thickBot="1">
       <c r="M33" s="11" t="s">
         <v>34</v>
       </c>
@@ -2523,12 +4798,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="13:21" ht="15" thickBot="1">
       <c r="M35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="13:21">
       <c r="M36" s="3"/>
       <c r="N36" s="3" t="s">
         <v>18</v>
@@ -2546,7 +4821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="13:21">
       <c r="M37" s="1" t="s">
         <v>14</v>
       </c>
@@ -2566,7 +4841,7 @@
         <v>6.4106238758192822E-5</v>
       </c>
     </row>
-    <row r="38" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="13:21">
       <c r="M38" s="1" t="s">
         <v>15</v>
       </c>
@@ -2582,7 +4857,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="13:21" ht="15" thickBot="1">
       <c r="M39" s="2" t="s">
         <v>16</v>
       </c>
@@ -2596,8 +4871,8 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="13:21" ht="15" thickBot="1"/>
+    <row r="41" spans="13:21">
       <c r="M41" s="3"/>
       <c r="N41" s="3" t="s">
         <v>23</v>
@@ -2624,7 +4899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="13:21">
       <c r="M42" s="1" t="s">
         <v>17</v>
       </c>
@@ -2653,7 +4928,7 @@
         <v>6.1383001761957994</v>
       </c>
     </row>
-    <row r="43" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="13:21">
       <c r="M43" s="1" t="s">
         <v>3</v>
       </c>
@@ -2682,7 +4957,7 @@
         <v>6.130467578064995E-2</v>
       </c>
     </row>
-    <row r="44" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="13:21" ht="15" thickBot="1">
       <c r="M44" s="2" t="s">
         <v>4</v>
       </c>
@@ -2711,13 +4986,13 @@
         <v>-6.9718984949400722E-3</v>
       </c>
     </row>
-    <row r="48" spans="13:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="13:21">
       <c r="M48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="50" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="13:15" ht="15" thickBot="1"/>
+    <row r="50" spans="13:15">
       <c r="M50" s="3" t="s">
         <v>38</v>
       </c>
@@ -2728,7 +5003,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="13:15">
       <c r="M51" s="1">
         <v>1</v>
       </c>
@@ -2739,7 +5014,7 @@
         <v>0.92285472538680047</v>
       </c>
     </row>
-    <row r="52" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="13:15">
       <c r="M52" s="1">
         <v>2</v>
       </c>
@@ -2750,7 +5025,7 @@
         <v>-0.5099895481070984</v>
       </c>
     </row>
-    <row r="53" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="13:15">
       <c r="M53" s="1">
         <v>3</v>
       </c>
@@ -2761,7 +5036,7 @@
         <v>1.5784302542944708</v>
       </c>
     </row>
-    <row r="54" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="13:15">
       <c r="M54" s="1">
         <v>4</v>
       </c>
@@ -2772,7 +5047,7 @@
         <v>-0.76348889666074449</v>
       </c>
     </row>
-    <row r="55" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="13:15">
       <c r="M55" s="1">
         <v>5</v>
       </c>
@@ -2783,7 +5058,7 @@
         <v>-0.30102540764971497</v>
       </c>
     </row>
-    <row r="56" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="13:15">
       <c r="M56" s="1">
         <v>6</v>
       </c>
@@ -2794,7 +5069,7 @@
         <v>1.2991873790782007</v>
       </c>
     </row>
-    <row r="57" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="13:15">
       <c r="M57" s="1">
         <v>7</v>
       </c>
@@ -2805,7 +5080,7 @@
         <v>-0.26806675960745796</v>
       </c>
     </row>
-    <row r="58" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="13:15">
       <c r="M58" s="1">
         <v>8</v>
       </c>
@@ -2816,7 +5091,7 @@
         <v>-0.29874169567993913</v>
       </c>
     </row>
-    <row r="59" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="13:15">
       <c r="M59" s="1">
         <v>9</v>
       </c>
@@ -2827,7 +5102,7 @@
         <v>-0.18883787866445179</v>
       </c>
     </row>
-    <row r="60" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="13:15">
       <c r="M60" s="1">
         <v>10</v>
       </c>
@@ -2838,7 +5113,7 @@
         <v>0.35325043332133887</v>
       </c>
     </row>
-    <row r="61" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="13:15">
       <c r="M61" s="1">
         <v>11</v>
       </c>
@@ -2849,7 +5124,7 @@
         <v>-0.40581732750488708</v>
       </c>
     </row>
-    <row r="62" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="13:15">
       <c r="M62" s="1">
         <v>12</v>
       </c>
@@ -2860,7 +5135,7 @@
         <v>-0.25116304680986001</v>
       </c>
     </row>
-    <row r="63" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="13:15">
       <c r="M63" s="1">
         <v>13</v>
       </c>
@@ -2871,7 +5146,7 @@
         <v>0.22241297005906535</v>
       </c>
     </row>
-    <row r="64" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="13:15">
       <c r="M64" s="1">
         <v>14</v>
       </c>
@@ -2882,7 +5157,7 @@
         <v>-1.1901793237169453</v>
       </c>
     </row>
-    <row r="65" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="13:15">
       <c r="M65" s="1">
         <v>15</v>
       </c>
@@ -2893,7 +5168,7 @@
         <v>2.3524471423883142E-2</v>
       </c>
     </row>
-    <row r="66" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="13:15">
       <c r="M66" s="1">
         <v>16</v>
       </c>
@@ -2904,7 +5179,7 @@
         <v>-0.23679210040127696</v>
       </c>
     </row>
-    <row r="67" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="13:15">
       <c r="M67" s="1">
         <v>17</v>
       </c>
@@ -2915,7 +5190,7 @@
         <v>-0.10418788141177959</v>
       </c>
     </row>
-    <row r="68" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="13:15">
       <c r="M68" s="1">
         <v>18</v>
       </c>
@@ -2926,7 +5201,7 @@
         <v>-0.23111210814614846</v>
       </c>
     </row>
-    <row r="69" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="13:15">
       <c r="M69" s="1">
         <v>19</v>
       </c>
@@ -2937,7 +5212,7 @@
         <v>0.72439448371397486</v>
       </c>
     </row>
-    <row r="70" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="13:15">
       <c r="M70" s="1">
         <v>20</v>
       </c>
@@ -2948,7 +5223,7 @@
         <v>0.38011420754473324</v>
       </c>
     </row>
-    <row r="71" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="13:15">
       <c r="M71" s="1">
         <v>21</v>
       </c>
@@ -2959,7 +5234,7 @@
         <v>-0.64138759159549164</v>
       </c>
     </row>
-    <row r="72" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="13:15">
       <c r="M72" s="1">
         <v>22</v>
       </c>
@@ -2970,7 +5245,7 @@
         <v>-0.21251976627910896</v>
       </c>
     </row>
-    <row r="73" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="13:15">
       <c r="M73" s="1">
         <v>23</v>
       </c>
@@ -2981,7 +5256,7 @@
         <v>0.58277040276034775</v>
       </c>
     </row>
-    <row r="74" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="13:15">
       <c r="M74" s="1">
         <v>24</v>
       </c>
@@ -2992,7 +5267,7 @@
         <v>-0.69979776780143599</v>
       </c>
     </row>
-    <row r="75" spans="13:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="13:15">
       <c r="M75" s="1">
         <v>25</v>
       </c>
@@ -3003,7 +5278,7 @@
         <v>0.60863981552020263</v>
       </c>
     </row>
-    <row r="76" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="13:15" ht="15" thickBot="1">
       <c r="M76" s="2">
         <v>26</v>
       </c>
@@ -3023,19 +5298,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A90CE2-368A-426F-91D3-A0D3271E0A90}">
-  <dimension ref="B1:O52"/>
+  <dimension ref="B1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12">
       <c r="B1" t="s">
         <v>41</v>
       </c>
@@ -3048,11 +5323,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="2:12">
       <c r="B2" s="5">
         <v>6.4318788273508103</v>
       </c>
@@ -3065,8 +5337,11 @@
       <c r="E2" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1">
       <c r="B3" s="5">
         <v>5.44441351714429</v>
       </c>
@@ -3079,12 +5354,8 @@
       <c r="E3" s="5">
         <v>6.3</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" s="5">
         <v>7.0755203181297501</v>
       </c>
@@ -3097,14 +5368,12 @@
       <c r="E4" s="5">
         <v>49.4</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="12">
-        <v>0.42133043146253152</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="5">
         <v>5.08566368146671</v>
       </c>
@@ -3118,13 +5387,13 @@
         <v>37.700000000000003</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="12">
-        <v>0.17751933247640295</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+        <v>0.66123510767858384</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" s="5">
         <v>4.7964451962038597</v>
       </c>
@@ -3138,13 +5407,13 @@
         <v>45.8</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="12">
-        <v>0.14324930466291974</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+        <v>0.43723186762670835</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="5">
         <v>6.8266932831903402</v>
       </c>
@@ -3158,13 +5427,13 @@
         <v>3.4</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="12">
-        <v>0.85133186092910684</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.36049075866671404</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="5">
         <v>5.4762647807990499</v>
       </c>
@@ -3177,14 +5446,14 @@
       <c r="E8" s="5">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="13">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0.73552098269578636</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1">
       <c r="B9" s="5">
         <v>4.7112028804681403</v>
       </c>
@@ -3197,8 +5466,14 @@
       <c r="E9" s="5">
         <v>34.1</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="5">
         <v>4.5613915516479304</v>
       </c>
@@ -3211,11 +5486,8 @@
       <c r="E10" s="5">
         <v>50.2</v>
       </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1">
       <c r="B11" s="5">
         <v>5.8605529925142203</v>
       </c>
@@ -3228,24 +5500,11 @@
       <c r="E11" s="5">
         <v>47.3</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
       <c r="B12" s="5">
         <v>5.0724921541501304</v>
       </c>
@@ -3258,26 +5517,24 @@
       <c r="E12" s="5">
         <v>10.1</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="12">
-        <v>3.754299999841944</v>
-      </c>
-      <c r="J12" s="12">
-        <v>3.754299999841944</v>
-      </c>
-      <c r="K12" s="12">
-        <v>5.1800171695968009</v>
-      </c>
-      <c r="L12" s="12">
-        <v>3.2060865142186257E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="5">
         <v>5.6985743637850597</v>
       </c>
@@ -3291,21 +5548,25 @@
         <v>21.3</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="12">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="I13" s="12">
-        <v>17.394382498392385</v>
+        <v>9.2468779465472757</v>
       </c>
       <c r="J13" s="12">
-        <v>0.72476593743301609</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>3.082292648849092</v>
+      </c>
+      <c r="K13" s="12">
+        <v>5.6974921727367844</v>
+      </c>
+      <c r="L13" s="12">
+        <v>4.8219367752981562E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
       <c r="B14" s="5">
         <v>7.6259972783801704</v>
       </c>
@@ -3318,20 +5579,22 @@
       <c r="E14" s="5">
         <v>19.399999999999999</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="13">
-        <v>25</v>
-      </c>
-      <c r="I14" s="13">
-        <v>21.148682498234329</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="12">
+        <v>22</v>
+      </c>
+      <c r="I14" s="12">
+        <v>11.901804551687054</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0.54099111598577521</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1">
       <c r="B15" s="5">
         <v>4.6735596734639602</v>
       </c>
@@ -3344,8 +5607,20 @@
       <c r="E15" s="5">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="13">
+        <v>25</v>
+      </c>
+      <c r="I15" s="13">
+        <v>21.148682498234329</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1">
       <c r="B16" s="5">
         <v>5.68095535436803</v>
       </c>
@@ -3358,33 +5633,8 @@
       <c r="E16" s="5">
         <v>27.8</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="2:15">
       <c r="B17" s="5">
         <v>4.8851347471210502</v>
       </c>
@@ -3397,35 +5647,33 @@
       <c r="E17" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="12">
-        <v>-2.0323342273268832</v>
-      </c>
-      <c r="I17" s="12">
-        <v>3.3400829315673151</v>
-      </c>
-      <c r="J17" s="12">
-        <v>-0.608468193444892</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0.54859306269530017</v>
-      </c>
-      <c r="L17" s="12">
-        <v>-8.925926585506982</v>
-      </c>
-      <c r="M17" s="12">
-        <v>4.8612581308532166</v>
-      </c>
-      <c r="N17" s="12">
-        <v>-8.925926585506982</v>
-      </c>
-      <c r="O17" s="12">
-        <v>4.8612581308532166</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G17" s="14"/>
+      <c r="H17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
       <c r="B18" s="5">
         <v>5.5941235954617596</v>
       </c>
@@ -3438,35 +5686,35 @@
       <c r="E18" s="5">
         <v>23.7</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="13">
-        <v>5.6942519302292056E-2</v>
-      </c>
-      <c r="I18" s="13">
-        <v>2.5019065151714884E-2</v>
-      </c>
-      <c r="J18" s="13">
-        <v>2.2759651072889526</v>
-      </c>
-      <c r="K18" s="13">
-        <v>3.2060865142186083E-2</v>
-      </c>
-      <c r="L18" s="13">
-        <v>5.3057067223898496E-3</v>
-      </c>
-      <c r="M18" s="13">
-        <v>0.10857933188219426</v>
-      </c>
-      <c r="N18" s="13">
-        <v>5.3057067223898496E-3</v>
-      </c>
-      <c r="O18" s="13">
-        <v>0.10857933188219426</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="12">
+        <v>-4.4305496742511448</v>
+      </c>
+      <c r="I18" s="12">
+        <v>3.2299787834386691</v>
+      </c>
+      <c r="J18" s="12">
+        <v>-1.3716962157671932</v>
+      </c>
+      <c r="K18" s="16">
+        <v>0.1839862176147424</v>
+      </c>
+      <c r="L18" s="12">
+        <v>-11.12911568312601</v>
+      </c>
+      <c r="M18" s="12">
+        <v>2.268016334623721</v>
+      </c>
+      <c r="N18" s="12">
+        <v>-11.12911568312601</v>
+      </c>
+      <c r="O18" s="12">
+        <v>2.268016334623721</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
       <c r="B19" s="5">
         <v>6.6452977800681898</v>
       </c>
@@ -3479,8 +5727,35 @@
       <c r="E19" s="5">
         <v>14.1</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="12">
+        <v>8.3812671827685675E-2</v>
+      </c>
+      <c r="I19" s="12">
+        <v>2.4353736288181129E-2</v>
+      </c>
+      <c r="J19" s="12">
+        <v>3.4414707803319677</v>
+      </c>
+      <c r="K19" s="16">
+        <v>2.3287539252376545E-3</v>
+      </c>
+      <c r="L19" s="12">
+        <v>3.3306114036789874E-2</v>
+      </c>
+      <c r="M19" s="12">
+        <v>0.13431922961858148</v>
+      </c>
+      <c r="N19" s="12">
+        <v>3.3306114036789874E-2</v>
+      </c>
+      <c r="O19" s="12">
+        <v>0.13431922961858148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
       <c r="B20" s="5">
         <v>5.41703052445233</v>
       </c>
@@ -3493,8 +5768,35 @@
       <c r="E20" s="5">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="12">
+        <v>-1.4765124149180849E-2</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1.1983151170237712E-2</v>
+      </c>
+      <c r="J20" s="12">
+        <v>-1.2321570461242835</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.23089754992460404</v>
+      </c>
+      <c r="L20" s="12">
+        <v>-3.9616658629759452E-2</v>
+      </c>
+      <c r="M20" s="12">
+        <v>1.008641033139775E-2</v>
+      </c>
+      <c r="N20" s="12">
+        <v>-3.9616658629759452E-2</v>
+      </c>
+      <c r="O20" s="12">
+        <v>1.008641033139775E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="15" thickBot="1">
       <c r="B21" s="5">
         <v>6.5047254855080299</v>
       </c>
@@ -3507,8 +5809,35 @@
       <c r="E21" s="5">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="13">
+        <v>-3.580278362975766E-2</v>
+      </c>
+      <c r="I21" s="13">
+        <v>1.1359266539318734E-2</v>
+      </c>
+      <c r="J21" s="13">
+        <v>-3.1518569888144303</v>
+      </c>
+      <c r="K21" s="17">
+        <v>4.6274105773091668E-3</v>
+      </c>
+      <c r="L21" s="13">
+        <v>-5.9360460576794144E-2</v>
+      </c>
+      <c r="M21" s="13">
+        <v>-1.2245106682721173E-2</v>
+      </c>
+      <c r="N21" s="13">
+        <v>-5.9360460576794144E-2</v>
+      </c>
+      <c r="O21" s="13">
+        <v>-1.2245106682721173E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
       <c r="B22" s="5">
         <v>3.9509466188803</v>
       </c>
@@ -3521,11 +5850,8 @@
       <c r="E22" s="5">
         <v>25.8</v>
       </c>
-      <c r="G22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="2:15">
       <c r="B23" s="5">
         <v>5.5779973997348504</v>
       </c>
@@ -3539,7 +5865,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:15">
       <c r="B24" s="5">
         <v>5.9792870175683399</v>
       </c>
@@ -3552,17 +5878,8 @@
       <c r="E24" s="5">
         <v>3.4</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="2:15">
       <c r="B25" s="5">
         <v>3.8006515546829598</v>
       </c>
@@ -3575,17 +5892,11 @@
       <c r="E25" s="5">
         <v>26.9</v>
       </c>
-      <c r="G25" s="12">
-        <v>1</v>
-      </c>
-      <c r="H25" s="12">
-        <v>5.3075565107385634</v>
-      </c>
-      <c r="I25" s="12">
-        <v>1.1243223166122469</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="2:15">
       <c r="B26" s="5">
         <v>5.3526167886391498</v>
       </c>
@@ -3598,17 +5909,11 @@
       <c r="E26" s="5">
         <v>22.2</v>
       </c>
-      <c r="G26" s="12">
-        <v>2</v>
-      </c>
-      <c r="H26" s="12">
-        <v>5.6036576111104814</v>
-      </c>
-      <c r="I26" s="12">
-        <v>-0.15924409396619144</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="2:15">
       <c r="B27" s="5">
         <v>5.8325243895774301</v>
       </c>
@@ -3621,282 +5926,448 @@
       <c r="E27" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G27" s="12">
-        <v>3</v>
-      </c>
-      <c r="H27" s="12">
-        <v>5.9567012307846934</v>
-      </c>
-      <c r="I27" s="12">
-        <v>1.1188190873450568</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G28" s="12">
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="15" thickBot="1"/>
+    <row r="29" spans="2:15">
+      <c r="G29" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="G30" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.63118576456147546</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="12">
-        <v>5.768790917087129</v>
-      </c>
-      <c r="I28" s="12">
-        <v>-0.68312723562041899</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G29" s="12">
-        <v>5</v>
-      </c>
-      <c r="H29" s="12">
-        <v>5.8997587114824013</v>
-      </c>
-      <c r="I29" s="12">
-        <v>-1.1033135152785416</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G30" s="12">
-        <v>6</v>
-      </c>
-      <c r="H30" s="12">
-        <v>5.6662943823430023</v>
-      </c>
-      <c r="I30" s="12">
-        <v>1.1603989008473379</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G31" s="12">
-        <v>7</v>
+      <c r="G31" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="H31" s="12">
-        <v>5.3132507626687921</v>
-      </c>
-      <c r="I31" s="12">
-        <v>0.16301401813025773</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G32" s="12">
-        <v>8</v>
+        <v>0.39839546938505432</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="C32" s="5">
+        <v>128.9</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="H32" s="12">
-        <v>5.9225357192033163</v>
-      </c>
-      <c r="I32" s="12">
-        <v>-1.2113328387351761</v>
-      </c>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G33" s="12">
-        <v>9</v>
+        <v>0.34608203194027648</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15">
+      <c r="C33" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D33" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="H33" s="12">
-        <v>5.4043587935524586</v>
-      </c>
-      <c r="I33" s="12">
-        <v>-0.84296724190452821</v>
-      </c>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G34" s="12">
-        <v>10</v>
-      </c>
-      <c r="H34" s="12">
-        <v>6.2528023311566105</v>
-      </c>
-      <c r="I34" s="12">
-        <v>-0.3922493386423902</v>
-      </c>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G35" s="12">
+        <v>0.74376080795873156</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" ht="15" thickBot="1">
+      <c r="C34" s="5">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="D34" s="5">
+        <v>49.4</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15">
+      <c r="C35" s="5">
+        <v>137</v>
+      </c>
+      <c r="D35" s="5">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" ht="15" thickBot="1">
+      <c r="C36" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D36" s="5">
+        <v>45.8</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15">
+      <c r="C37" s="5">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15">
+      <c r="C38" s="5">
+        <v>129</v>
+      </c>
+      <c r="D38" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="12">
+        <v>2</v>
+      </c>
+      <c r="I38" s="12">
+        <v>8.4255392907595485</v>
+      </c>
+      <c r="J38" s="12">
+        <v>4.2127696453797743</v>
+      </c>
+      <c r="K38" s="12">
+        <v>7.6155475312743679</v>
+      </c>
+      <c r="L38" s="12">
+        <v>2.8978615299427839E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15">
+      <c r="C39" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="D39" s="5">
+        <v>34.1</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="12">
+        <v>23</v>
+      </c>
+      <c r="I39" s="12">
+        <v>12.723143207474781</v>
+      </c>
+      <c r="J39" s="12">
+        <v>0.55318013945542521</v>
+      </c>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+    </row>
+    <row r="40" spans="3:15" ht="15" thickBot="1">
+      <c r="C40" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="D40" s="5">
+        <v>50.2</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="13">
+        <v>25</v>
+      </c>
+      <c r="I40" s="13">
+        <v>21.148682498234329</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="3:15" ht="15" thickBot="1">
+      <c r="C41" s="5">
+        <v>145.5</v>
+      </c>
+      <c r="D41" s="5">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15">
+      <c r="C42" s="5">
+        <v>128.9</v>
+      </c>
+      <c r="D42" s="5">
+        <v>10.1</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="12">
-        <v>5.3075565107385634</v>
-      </c>
-      <c r="I35" s="12">
-        <v>-0.23506435658843294</v>
-      </c>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G36" s="12">
-        <v>12</v>
-      </c>
-      <c r="H36" s="12">
-        <v>5.6036576111104814</v>
-      </c>
-      <c r="I36" s="12">
-        <v>9.491675267457822E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G37" s="12">
-        <v>13</v>
-      </c>
-      <c r="H37" s="12">
-        <v>5.9567012307846934</v>
-      </c>
-      <c r="I37" s="12">
-        <v>1.669296047595477</v>
-      </c>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G38" s="12">
-        <v>14</v>
-      </c>
-      <c r="H38" s="12">
-        <v>5.768790917087129</v>
-      </c>
-      <c r="I38" s="12">
-        <v>-1.0952312436231688</v>
-      </c>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G39" s="12">
-        <v>15</v>
-      </c>
-      <c r="H39" s="12">
-        <v>5.8997587114824013</v>
-      </c>
-      <c r="I39" s="12">
-        <v>-0.21880335711437127</v>
-      </c>
-    </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G40" s="12">
-        <v>16</v>
-      </c>
-      <c r="H40" s="12">
-        <v>5.6662943823430023</v>
-      </c>
-      <c r="I40" s="12">
-        <v>-0.78115963522195209</v>
-      </c>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G41" s="12">
+      <c r="J42" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K42" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O42" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15">
+      <c r="C43" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D43" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="G43" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="12">
-        <v>5.3132507626687921</v>
-      </c>
-      <c r="I41" s="12">
-        <v>0.28087283279296749</v>
-      </c>
-    </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G42" s="12">
-        <v>18</v>
-      </c>
-      <c r="H42" s="12">
-        <v>5.9225357192033163</v>
-      </c>
-      <c r="I42" s="12">
-        <v>0.72276206086487349</v>
-      </c>
-    </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G43" s="12">
-        <v>19</v>
-      </c>
       <c r="H43" s="12">
-        <v>5.4043587935524586</v>
+        <v>-5.4815519817074412</v>
       </c>
       <c r="I43" s="12">
-        <v>1.2671730899871392E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G44" s="12">
-        <v>20</v>
+        <v>3.1502157171428937</v>
+      </c>
+      <c r="J43" s="12">
+        <v>-1.740056070407447</v>
+      </c>
+      <c r="K43" s="12">
+        <v>9.5215123303993343E-2</v>
+      </c>
+      <c r="L43" s="12">
+        <v>-11.99826969943679</v>
+      </c>
+      <c r="M43" s="12">
+        <v>1.0351657360219084</v>
+      </c>
+      <c r="N43" s="12">
+        <v>-11.99826969943679</v>
+      </c>
+      <c r="O43" s="12">
+        <v>1.0351657360219084</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15">
+      <c r="C44" s="5">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="D44" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="H44" s="12">
-        <v>6.2528023311566105</v>
+        <v>8.820298806516802E-2</v>
       </c>
       <c r="I44" s="12">
-        <v>0.25192315435141932</v>
-      </c>
-    </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G45" s="12">
-        <v>21</v>
-      </c>
-      <c r="H45" s="12">
-        <v>4.8064623408783929</v>
-      </c>
-      <c r="I45" s="12">
-        <v>-0.85551572199809289</v>
-      </c>
-    </row>
-    <row r="46" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G46" s="12">
-        <v>22</v>
-      </c>
-      <c r="H46" s="12">
-        <v>5.1538117086223743</v>
-      </c>
-      <c r="I46" s="12">
-        <v>0.42418569111247617</v>
-      </c>
-    </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G47" s="12">
-        <v>23</v>
-      </c>
-      <c r="H47" s="12">
-        <v>5.1310347009014574</v>
-      </c>
-      <c r="I47" s="12">
-        <v>0.8482523166668825</v>
-      </c>
-    </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G48" s="12">
-        <v>24</v>
-      </c>
-      <c r="H48" s="12">
-        <v>5.1424232047619158</v>
-      </c>
-      <c r="I48" s="12">
-        <v>-1.341771650078956</v>
-      </c>
-    </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G49" s="12">
-        <v>25</v>
-      </c>
-      <c r="H49" s="12">
-        <v>5.0627036777387069</v>
-      </c>
-      <c r="I49" s="12">
-        <v>0.28991311090044292</v>
-      </c>
-    </row>
-    <row r="50" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G50" s="13">
-        <v>26</v>
-      </c>
-      <c r="H50" s="13">
-        <v>5.0740921815991653</v>
-      </c>
-      <c r="I50" s="13">
-        <v>0.75843220797826483</v>
-      </c>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-    </row>
-    <row r="52" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
+        <v>2.4361564521045258E-2</v>
+      </c>
+      <c r="J44" s="12">
+        <v>3.6205797862026468</v>
+      </c>
+      <c r="K44" s="12">
+        <v>1.4357700339917741E-3</v>
+      </c>
+      <c r="L44" s="12">
+        <v>3.7807252216993055E-2</v>
+      </c>
+      <c r="M44" s="12">
+        <v>0.13859872391334299</v>
+      </c>
+      <c r="N44" s="12">
+        <v>3.7807252216993055E-2</v>
+      </c>
+      <c r="O44" s="12">
+        <v>0.13859872391334299</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" ht="15" thickBot="1">
+      <c r="C45" s="5">
+        <v>137</v>
+      </c>
+      <c r="D45" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="13">
+        <v>-3.2342975335469058E-2</v>
+      </c>
+      <c r="I45" s="13">
+        <v>1.1130052213117754E-2</v>
+      </c>
+      <c r="J45" s="13">
+        <v>-2.9059140708567379</v>
+      </c>
+      <c r="K45" s="13">
+        <v>7.9615387845873263E-3</v>
+      </c>
+      <c r="L45" s="13">
+        <v>-5.5367242550496479E-2</v>
+      </c>
+      <c r="M45" s="13">
+        <v>-9.3187081204416378E-3</v>
+      </c>
+      <c r="N45" s="13">
+        <v>-5.5367242550496479E-2</v>
+      </c>
+      <c r="O45" s="13">
+        <v>-9.3187081204416378E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15">
+      <c r="C46" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D46" s="5">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15">
+      <c r="C47" s="5">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="D47" s="5">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15">
+      <c r="C48" s="5">
+        <v>129</v>
+      </c>
+      <c r="D48" s="5">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9">
+      <c r="C49" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="D49" s="5">
+        <v>14.1</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="3:9" ht="15" thickBot="1">
+      <c r="C50" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="D50" s="5">
+        <v>25.2</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="3:9">
+      <c r="C51" s="5">
+        <v>145.5</v>
+      </c>
+      <c r="D51" s="5">
+        <v>25.3</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="3:9" ht="15" thickBot="1">
+      <c r="C52" s="5">
+        <v>120.1</v>
+      </c>
+      <c r="D52" s="5">
+        <v>25.8</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="3:9">
+      <c r="C53" s="5">
+        <v>126.2</v>
+      </c>
+      <c r="D53" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9">
+      <c r="C54" s="5">
+        <v>125.8</v>
+      </c>
+      <c r="D54" s="5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9">
+      <c r="C55" s="5">
+        <v>126</v>
+      </c>
+      <c r="D55" s="5">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9">
+      <c r="C56" s="5">
+        <v>124.6</v>
+      </c>
+      <c r="D56" s="5">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9">
+      <c r="C57" s="5">
+        <v>124.8</v>
+      </c>
+      <c r="D57" s="5">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>